<commit_message>
Refinação UML e Espedificaçoes
Pequenas alterações em ambos
</commit_message>
<xml_diff>
--- a/Especificação do gestor de notificações.xlsx
+++ b/Especificação do gestor de notificações.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="82">
   <si>
     <t>Nome</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Associa a nova notificação com destinatário</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>8.3</t>
+  </si>
+  <si>
+    <t>(volta a 3)</t>
   </si>
 </sst>
 </file>
@@ -380,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -730,17 +739,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -760,11 +758,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -782,158 +806,192 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1214,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,65 +1294,65 @@
       <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="27"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
+      <c r="B7" s="81"/>
       <c r="C7" s="5">
         <v>1</v>
       </c>
@@ -1306,12 +1364,12 @@
       <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="83" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
+      <c r="B8" s="81"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5">
@@ -1323,10 +1381,10 @@
       <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="38"/>
+      <c r="H8" s="83"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="41"/>
+      <c r="B9" s="81"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5">
@@ -1338,10 +1396,10 @@
       <c r="G9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="38"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="41"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="3">
         <v>4</v>
       </c>
@@ -1353,12 +1411,12 @@
       <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="73" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="41"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3">
@@ -1370,10 +1428,10 @@
       <c r="G11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="40"/>
+      <c r="H11" s="74"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="41"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3">
@@ -1385,10 +1443,10 @@
       <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="40"/>
+      <c r="H12" s="74"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="41"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3">
@@ -1400,694 +1458,717 @@
       <c r="G13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="40"/>
+      <c r="H13" s="74"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="41"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="9"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9">
         <v>8</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="29" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="40"/>
+      <c r="H14" s="74"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46" t="s">
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="94" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="41"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="86" t="s">
+      <c r="B16" s="95"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="87" t="s">
+      <c r="F16" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="87"/>
-      <c r="H16" s="88"/>
-    </row>
-    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="31"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="47" t="s">
+      <c r="G16" s="93"/>
+      <c r="H16" s="96"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="95"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="93"/>
+      <c r="E17" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="79"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="G17" s="93"/>
+      <c r="H17" s="96"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="99"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="100" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="86"/>
+      <c r="H18" s="101"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46" t="s">
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="H19" s="107" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="47" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="93"/>
+      <c r="E20" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F20" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="79"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="G20" s="93"/>
+      <c r="H20" s="108"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="18"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="97" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="98"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="42" t="s">
+      <c r="C22" s="103"/>
+      <c r="D22" s="104"/>
+      <c r="E22" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="71" t="s">
+      <c r="F22" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="43"/>
-      <c r="H20" s="44" t="s">
+      <c r="G22" s="104"/>
+      <c r="H22" s="106" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="10" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="54"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F23" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G23" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="39"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="H23" s="89"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="18"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="84"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C26" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="61"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C27" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="64"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C28" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="24"/>
-    </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="64"/>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C29" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="27"/>
-    </row>
-    <row r="27" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="17" t="s">
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="67"/>
+    </row>
+    <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29" t="s">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29" t="s">
+      <c r="E30" s="17"/>
+      <c r="F30" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G30" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H30" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="41"/>
-      <c r="C28" s="5">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="81"/>
+      <c r="C31" s="5">
         <v>0</v>
       </c>
-      <c r="D28" s="70" t="s">
+      <c r="D31" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="32" t="s">
+      <c r="E31" s="5"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="70" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="41"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="81"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="5">
         <v>1</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="33"/>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="41"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5">
+      <c r="H32" s="71"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="81"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="5">
         <v>2</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="33"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="41"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5">
+      <c r="H33" s="71"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="81"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="5">
         <v>3</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="33"/>
-    </row>
-    <row r="32" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="41"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="49">
+      <c r="H34" s="71"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="81"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="24">
         <v>4</v>
       </c>
-      <c r="F32" s="50" t="s">
+      <c r="F35" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="50" t="s">
+      <c r="G35" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="33"/>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="49">
+      <c r="H35" s="71"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="82"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="24">
         <v>5</v>
       </c>
-      <c r="F33" s="56" t="s">
+      <c r="F36" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="50"/>
-      <c r="H33" s="51"/>
-    </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="14" t="s">
+      <c r="G36" s="25"/>
+      <c r="H36" s="79"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="26"/>
+      <c r="B38" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C38" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
-      <c r="I35" s="52"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="15" t="s">
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="61"/>
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="26"/>
+      <c r="B39" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C39" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="24"/>
-      <c r="I36" s="52"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="15" t="s">
+      <c r="D39" s="63"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="64"/>
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="26"/>
+      <c r="B40" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C40" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="24"/>
-      <c r="I37" s="52"/>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="52"/>
-      <c r="B38" s="16" t="s">
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="64"/>
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26"/>
+      <c r="B41" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C41" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="27"/>
-      <c r="I38" s="52"/>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
-      <c r="B39" s="54" t="s">
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="26"/>
+      <c r="B42" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="53"/>
-      <c r="D39" s="29" t="s">
+      <c r="C42" s="27"/>
+      <c r="D42" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29" t="s">
+      <c r="E42" s="17"/>
+      <c r="F42" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G42" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="37" t="s">
+      <c r="H42" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="52"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
-      <c r="B40" s="55"/>
-      <c r="C40" s="12">
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="26"/>
+      <c r="B43" s="69"/>
+      <c r="C43" s="12">
         <v>1</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="5"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
+      <c r="E43" s="5"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H40" s="32" t="s">
+      <c r="H43" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="52"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="55"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5">
+      <c r="I43" s="26"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="26"/>
+      <c r="B44" s="69"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5">
         <v>2</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="G44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H41" s="33"/>
-      <c r="I41" s="52"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="5">
+      <c r="H44" s="71"/>
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="26"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5">
         <v>3</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="33"/>
-      <c r="I42" s="52"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="52"/>
-      <c r="B43" s="55"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5">
+      <c r="H45" s="71"/>
+      <c r="I45" s="26"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="B46" s="69"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5">
         <v>4</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G43" s="4" t="s">
+      <c r="G46" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H43" s="34"/>
-      <c r="I43" s="52"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
-      <c r="B44" s="55"/>
-      <c r="C44" s="13">
+      <c r="H46" s="72"/>
+      <c r="I46" s="26"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="26"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="13">
         <v>5</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2" t="s">
+      <c r="E47" s="3"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H44" s="35" t="s">
+      <c r="H47" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="I44" s="52"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
-      <c r="B45" s="55"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="3">
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="26"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="3">
         <v>6</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="40"/>
-      <c r="I45" s="52"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="52"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="3">
+      <c r="H48" s="74"/>
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="26"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="3">
         <v>7</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F49" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="36"/>
-      <c r="I46" s="52"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="52"/>
-      <c r="B47" s="55"/>
-      <c r="C47" s="58">
+      <c r="H49" s="75"/>
+      <c r="I49" s="26"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="26"/>
+      <c r="B50" s="69"/>
+      <c r="C50" s="30">
         <v>8</v>
       </c>
-      <c r="D47" s="59" t="s">
+      <c r="D50" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="E47" s="62"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="60" t="s">
+      <c r="E50" s="33"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="H47" s="61" t="s">
+      <c r="H50" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="I47" s="52"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
-      <c r="B48" s="55"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="62">
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="26"/>
+      <c r="B51" s="69"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="33">
         <v>9</v>
       </c>
-      <c r="F48" s="59" t="s">
+      <c r="F51" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G48" s="60" t="s">
+      <c r="G51" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="63"/>
-      <c r="I48" s="52"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
-      <c r="B49" s="55"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="62">
+      <c r="H51" s="77"/>
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="26"/>
+      <c r="B52" s="69"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="33">
         <v>10</v>
       </c>
-      <c r="F49" s="59" t="s">
+      <c r="F52" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G49" s="60" t="s">
+      <c r="G52" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="64"/>
-      <c r="I49" s="52"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="52"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="65">
+      <c r="H52" s="78"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="69"/>
+      <c r="C53" s="34">
         <v>11</v>
       </c>
-      <c r="D50" s="66" t="s">
+      <c r="D53" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="E50" s="68"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66" t="s">
+      <c r="E53" s="36"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="H50" s="67" t="s">
+      <c r="H53" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="I50" s="52"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="52"/>
-      <c r="B51" s="55"/>
-      <c r="C51" s="65"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="68">
+      <c r="I53" s="26"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
+      <c r="B54" s="69"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="36">
         <v>12</v>
       </c>
-      <c r="F51" s="66" t="s">
+      <c r="F54" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="G51" s="66" t="s">
+      <c r="G54" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H51" s="69"/>
-      <c r="I51" s="52"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="52"/>
-      <c r="B52" s="55"/>
-      <c r="C52" s="65"/>
-      <c r="D52" s="66"/>
-      <c r="E52" s="68">
+      <c r="H54" s="52"/>
+      <c r="I54" s="26"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="36">
         <v>13</v>
       </c>
-      <c r="F52" s="66" t="s">
+      <c r="F55" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="G52" s="66" t="s">
+      <c r="G55" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="69"/>
-      <c r="I52" s="52"/>
-    </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="52"/>
-      <c r="B53" s="55"/>
-      <c r="C53" s="74"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="76">
+      <c r="H55" s="52"/>
+      <c r="I55" s="26"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="26"/>
+      <c r="B56" s="69"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="42">
         <v>14</v>
       </c>
-      <c r="F53" s="77" t="s">
+      <c r="F56" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="G53" s="75"/>
-      <c r="H53" s="69"/>
-      <c r="I53" s="52"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="52"/>
-      <c r="B54" s="28" t="s">
+      <c r="G56" s="41"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="26"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="26"/>
+      <c r="B57" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="91" t="s">
+      <c r="C57" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="D54" s="90" t="s">
+      <c r="D57" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="91"/>
-      <c r="F54" s="92"/>
-      <c r="G54" s="92"/>
-      <c r="H54" s="83" t="s">
+      <c r="E57" s="49"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="I54" s="52"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="52"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="73"/>
-      <c r="D55" s="72"/>
-      <c r="E55" s="73" t="s">
+      <c r="I57" s="26"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="26"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="38"/>
+      <c r="E58" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="F55" s="72" t="s">
+      <c r="F58" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="G55" s="72" t="s">
+      <c r="G58" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H55" s="84"/>
-      <c r="I55" s="52"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="52"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="72"/>
-      <c r="E56" s="73" t="s">
+      <c r="H58" s="57"/>
+      <c r="I58" s="26"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="26"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="38"/>
+      <c r="E59" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="72" t="s">
+      <c r="F59" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G56" s="72" t="s">
+      <c r="G59" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="H56" s="84"/>
-      <c r="I56" s="52"/>
-    </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="52"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="80"/>
-      <c r="E57" s="82" t="s">
+      <c r="H59" s="57"/>
+      <c r="I59" s="26"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="26"/>
+      <c r="B60" s="55"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="81" t="s">
+      <c r="F60" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="G57" s="80"/>
-      <c r="H57" s="85"/>
-      <c r="I57" s="52"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="1"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="89"/>
-      <c r="G59" s="89"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="G60" s="44"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="26"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C61" s="1"/>
@@ -2095,7 +2176,9 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C62" s="1"/>
-      <c r="E62" s="1"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1"/>
@@ -2242,12 +2325,15 @@
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C100" s="1"/>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C101" s="1"/>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="3:5" x14ac:dyDescent="0.25">
@@ -2421,38 +2507,45 @@
     <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" s="1"/>
     </row>
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E159" s="1"/>
+    </row>
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E160" s="1"/>
+    </row>
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E161" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="H50:H53"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H54:H57"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="B39:B53"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="H44:H46"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="H28:H33"/>
-    <mergeCell ref="B27:B33"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
+  <mergeCells count="28">
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="B6:B14"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="H53:H56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="B42:B56"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H50:H52"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="H31:H36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>